<commit_message>
Some updates on capacity expansion and offshore
- Zonal capacity expansion
- Extending nodal model with offshore wind investments
</commit_message>
<xml_diff>
--- a/data_sources/offshore_wind_farms.xlsx
+++ b/data_sources/offshore_wind_farms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hergun/Julia files/EU_grid_operations/data_sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3167666-8E13-A344-AC30-33275FEB8739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378D1E45-DA51-5448-92F3-26D1EC6E4498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15680" yWindow="-28300" windowWidth="24840" windowHeight="28300" xr2:uid="{29D019E9-3936-0C48-9DF2-44D2B22FF9DA}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{29D019E9-3936-0C48-9DF2-44D2B22FF9DA}"/>
   </bookViews>
   <sheets>
     <sheet name="OWFHUBS" sheetId="1" r:id="rId1"/>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A182882-2AAF-7A4F-9139-D1A45E91F100}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,7 +492,7 @@
         <v>53.425293000000003</v>
       </c>
       <c r="D5">
-        <v>1.6197889999999999</v>
+        <v>2.6197889999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -506,7 +506,7 @@
         <v>54.110849999999999</v>
       </c>
       <c r="D6">
-        <v>0.993425</v>
+        <v>1.993425</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -520,7 +520,7 @@
         <v>54.905489000000003</v>
       </c>
       <c r="D7">
-        <v>0.29746499999999998</v>
+        <v>2.7974649999999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -534,7 +534,7 @@
         <v>55.540615000000003</v>
       </c>
       <c r="D8">
-        <v>-0.46809200000000001</v>
+        <v>2.468092</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -548,7 +548,7 @@
         <v>56.152724999999997</v>
       </c>
       <c r="D9">
-        <v>-0.86246900000000004</v>
+        <v>1.8624689999999999</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -562,7 +562,7 @@
         <v>56.767954000000003</v>
       </c>
       <c r="D10">
-        <v>-1.488834</v>
+        <v>1.488834</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -576,7 +576,7 @@
         <v>57.448231999999997</v>
       </c>
       <c r="D11">
-        <v>-1.0480590000000001</v>
+        <v>1.0480590000000001</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -590,7 +590,7 @@
         <v>57.046612000000003</v>
       </c>
       <c r="D12">
-        <v>0.135074</v>
+        <v>1.1350739999999999</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -604,7 +604,7 @@
         <v>56.165644</v>
       </c>
       <c r="D13">
-        <v>0.94702799999999998</v>
+        <v>1.947028</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -618,7 +618,7 @@
         <v>55.528615000000002</v>
       </c>
       <c r="D14">
-        <v>0.327318</v>
+        <v>1.327318</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -632,7 +632,7 @@
         <v>54.989536999999999</v>
       </c>
       <c r="D15">
-        <v>0.80996599999999996</v>
+        <v>1.809966</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -646,7 +646,7 @@
         <v>54.443120999999998</v>
       </c>
       <c r="D16">
-        <v>1.64012</v>
+        <v>2.64012</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -758,7 +758,7 @@
         <v>56.725071</v>
       </c>
       <c r="D24">
-        <v>-5.1499000000000003E-2</v>
+        <v>2.0514990000000002</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -772,7 +772,7 @@
         <v>57.713828999999997</v>
       </c>
       <c r="D25">
-        <v>-0.51386699999999996</v>
+        <v>1.5138670000000001</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -786,7 +786,7 @@
         <v>58.628193000000003</v>
       </c>
       <c r="D26">
-        <v>-1.0918270000000001</v>
+        <v>1.0918270000000001</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -842,7 +842,7 @@
         <v>51.982000999999997</v>
       </c>
       <c r="D30">
-        <v>3.607615</v>
+        <v>4.607615</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -856,7 +856,7 @@
         <v>52.830095999999998</v>
       </c>
       <c r="D31">
-        <v>3.7489949999999999</v>
+        <v>4.7489949999999999</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -926,7 +926,7 @@
         <v>57.148130999999999</v>
       </c>
       <c r="D36">
-        <v>7.2382090000000003</v>
+        <v>6.2382090000000003</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -940,7 +940,7 @@
         <v>56.253177999999998</v>
       </c>
       <c r="D37">
-        <v>7.1880490000000004</v>
+        <v>6.1880490000000004</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -954,7 +954,7 @@
         <v>55.495677999999998</v>
       </c>
       <c r="D38">
-        <v>7.4708839999999999</v>
+        <v>6.4708839999999999</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -968,7 +968,7 @@
         <v>54.994207000000003</v>
       </c>
       <c r="D39">
-        <v>7.7550889999999999</v>
+        <v>6.7550889999999999</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1010,7 +1010,7 @@
         <v>53.836644</v>
       </c>
       <c r="D42">
-        <v>7.2949479999999998</v>
+        <v>6.2949479999999998</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1024,7 +1024,7 @@
         <v>53.977496000000002</v>
       </c>
       <c r="D43">
-        <v>7.9680590000000002</v>
+        <v>6.9680590000000002</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1038,7 +1038,7 @@
         <v>54.033403</v>
       </c>
       <c r="D44">
-        <v>8.4278340000000007</v>
+        <v>7.4278339999999998</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1052,7 +1052,7 @@
         <v>54.441091</v>
       </c>
       <c r="D45">
-        <v>8.1741650000000003</v>
+        <v>7.1741650000000003</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1066,7 +1066,7 @@
         <v>54.293194</v>
       </c>
       <c r="D46">
-        <v>6.5419450000000001</v>
+        <v>5.5419450000000001</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1080,7 +1080,7 @@
         <v>54.893127</v>
       </c>
       <c r="D47">
-        <v>6.6296989999999996</v>
+        <v>5.6296989999999996</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1094,7 +1094,7 @@
         <v>54.487358</v>
       </c>
       <c r="D48">
-        <v>5.295833</v>
+        <v>4.295833</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1108,7 +1108,7 @@
         <v>54.548482</v>
       </c>
       <c r="D49">
-        <v>6.4366390000000004</v>
+        <v>5.4366390000000004</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1122,7 +1122,7 @@
         <v>55.174757</v>
       </c>
       <c r="D50">
-        <v>6.8403090000000004</v>
+        <v>5.8403090000000004</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1136,7 +1136,7 @@
         <v>54.660305999999999</v>
       </c>
       <c r="D51">
-        <v>7.2790809999999997</v>
+        <v>6.2790809999999997</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1150,7 +1150,7 @@
         <v>54.872934999999998</v>
       </c>
       <c r="D52">
-        <v>5.1905279999999996</v>
+        <v>4.1905279999999996</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1164,7 +1164,7 @@
         <v>55.37471</v>
       </c>
       <c r="D53">
-        <v>5.8048080000000004</v>
+        <v>4.8048080000000004</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1178,7 +1178,7 @@
         <v>55.134644999999999</v>
       </c>
       <c r="D54">
-        <v>5.0852219999999999</v>
+        <v>4.0852219999999999</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1192,7 +1192,7 @@
         <v>54.619678</v>
       </c>
       <c r="D55">
-        <v>5.0501209999999999</v>
+        <v>4.0501209999999999</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1206,7 +1206,7 @@
         <v>55.394651000000003</v>
       </c>
       <c r="D56">
-        <v>5.295833</v>
+        <v>4.295833</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1220,7 +1220,7 @@
         <v>55.558771999999998</v>
       </c>
       <c r="D57">
-        <v>4.4446159999999999</v>
+        <v>3.4446159999999999</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1234,7 +1234,7 @@
         <v>54.888080000000002</v>
       </c>
       <c r="D58">
-        <v>4.5499210000000003</v>
+        <v>3.5499209999999999</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1248,7 +1248,7 @@
         <v>54.489905999999998</v>
       </c>
       <c r="D59">
-        <v>4.8438980000000003</v>
+        <v>3.8438979999999998</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1262,7 +1262,7 @@
         <v>54.093698000000003</v>
       </c>
       <c r="D60">
-        <v>5.0424220000000002</v>
+        <v>4.0424220000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>